<commit_message>
finishing exporting database tables into dBase files
</commit_message>
<xml_diff>
--- a/prj/2/ACS_16_5YR_S1901_with_ann.xlsx
+++ b/prj/2/ACS_16_5YR_S1901_with_ann.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Admin\Desktop\CompSci\CMPT220-Lin\prj\2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B43BB34D-80F0-4345-AA6A-9DE6E112D2E9}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{7315DF4E-6AA0-4F9C-8CF3-6B2E68F1DDCA}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15345" windowHeight="4455"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7545"/>
   </bookViews>
   <sheets>
     <sheet name="ACS_16_5YR_S1901_with_ann" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+  <si>
+    <t>CITY</t>
+  </si>
+  <si>
+    <t>STATE</t>
+  </si>
   <si>
     <t>Households; Estimate; Total</t>
   </si>
@@ -34,6 +40,30 @@
     <t>Nonfamily households; Estimate; Total</t>
   </si>
   <si>
+    <t>Households; Estimate; Median income (dollars)</t>
+  </si>
+  <si>
+    <t>Families; Estimate; Median income (dollars)</t>
+  </si>
+  <si>
+    <t>Married-couple families; Estimate; Median income (dollars)</t>
+  </si>
+  <si>
+    <t>Nonfamily households; Estimate; Median income (dollars)</t>
+  </si>
+  <si>
+    <t>Households; Estimate; Mean income (dollars)</t>
+  </si>
+  <si>
+    <t>Families; Estimate; Mean income (dollars)</t>
+  </si>
+  <si>
+    <t>Married-couple families; Estimate; Mean income (dollars)</t>
+  </si>
+  <si>
+    <t>Nonfamily households; Estimate; Mean income (dollars)</t>
+  </si>
+  <si>
     <t>Households; Estimate; Less than $10,000</t>
   </si>
   <si>
@@ -154,34 +184,7 @@
     <t>Nonfamily households; Estimate; $200,000 or more</t>
   </si>
   <si>
-    <t>Households; Estimate; Median income (dollars)</t>
-  </si>
-  <si>
-    <t>Families; Estimate; Median income (dollars)</t>
-  </si>
-  <si>
-    <t>Married-couple families; Estimate; Median income (dollars)</t>
-  </si>
-  <si>
-    <t>Nonfamily households; Estimate; Median income (dollars)</t>
-  </si>
-  <si>
-    <t>Households; Estimate; Mean income (dollars)</t>
-  </si>
-  <si>
-    <t>Families; Estimate; Mean income (dollars)</t>
-  </si>
-  <si>
-    <t>Married-couple families; Estimate; Mean income (dollars)</t>
-  </si>
-  <si>
-    <t>Nonfamily households; Estimate; Mean income (dollars)</t>
-  </si>
-  <si>
-    <t>CITY</t>
-  </si>
-  <si>
-    <t>STATE</t>
+    <t>FAMILY_COST_OF_LIVING</t>
   </si>
   <si>
     <t>Miami city</t>
@@ -194,7 +197,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -329,6 +332,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -511,7 +524,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -626,8 +639,23 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="22"/>
+      </left>
+      <right style="thin">
+        <color indexed="22"/>
+      </right>
+      <top style="thin">
+        <color indexed="22"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="22"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="42">
+  <cellStyleXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -670,11 +698,18 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="42" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="42">
+  <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -712,6 +747,7 @@
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal_ACS_16_5YR_S1901_with_ann" xfId="42"/>
     <cellStyle name="Note" xfId="15" builtinId="10" customBuiltin="1"/>
     <cellStyle name="Output" xfId="10" builtinId="21" customBuiltin="1"/>
     <cellStyle name="Title" xfId="1" builtinId="15" customBuiltin="1"/>
@@ -1028,190 +1064,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BB2"/>
+  <dimension ref="A1:BC3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="25.42578125" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
-    <col min="5" max="5" width="36.28515625" customWidth="1"/>
-    <col min="6" max="6" width="35.42578125" customWidth="1"/>
+    <col min="2" max="2" width="10.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+      <c r="AD1" t="s">
+        <v>29</v>
+      </c>
+      <c r="AE1" t="s">
+        <v>30</v>
+      </c>
+      <c r="AF1" t="s">
+        <v>31</v>
+      </c>
+      <c r="AG1" t="s">
+        <v>32</v>
+      </c>
+      <c r="AH1" t="s">
+        <v>33</v>
+      </c>
+      <c r="AI1" t="s">
+        <v>34</v>
+      </c>
+      <c r="AJ1" t="s">
+        <v>35</v>
+      </c>
+      <c r="AK1" t="s">
+        <v>36</v>
+      </c>
+      <c r="AL1" t="s">
+        <v>37</v>
+      </c>
+      <c r="AM1" t="s">
+        <v>38</v>
+      </c>
+      <c r="AN1" t="s">
+        <v>39</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>40</v>
+      </c>
+      <c r="AP1" t="s">
+        <v>41</v>
+      </c>
+      <c r="AQ1" t="s">
+        <v>42</v>
+      </c>
+      <c r="AR1" t="s">
+        <v>43</v>
+      </c>
+      <c r="AS1" t="s">
+        <v>44</v>
+      </c>
+      <c r="AT1" t="s">
+        <v>45</v>
+      </c>
+      <c r="AU1" t="s">
+        <v>46</v>
+      </c>
+      <c r="AV1" t="s">
+        <v>47</v>
+      </c>
+      <c r="AW1" t="s">
+        <v>48</v>
+      </c>
+      <c r="AX1" t="s">
+        <v>49</v>
+      </c>
+      <c r="AY1" t="s">
+        <v>50</v>
+      </c>
+      <c r="AZ1" t="s">
+        <v>51</v>
+      </c>
+      <c r="BA1" t="s">
         <v>52</v>
       </c>
-      <c r="B1" t="s">
+      <c r="BB1" t="s">
         <v>53</v>
       </c>
-      <c r="C1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J1" t="s">
-        <v>47</v>
-      </c>
-      <c r="K1" t="s">
-        <v>48</v>
-      </c>
-      <c r="L1" t="s">
-        <v>49</v>
-      </c>
-      <c r="M1" t="s">
-        <v>50</v>
-      </c>
-      <c r="N1" t="s">
-        <v>51</v>
-      </c>
-      <c r="O1" t="s">
-        <v>4</v>
-      </c>
-      <c r="P1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>6</v>
-      </c>
-      <c r="R1" t="s">
-        <v>7</v>
-      </c>
-      <c r="S1" t="s">
-        <v>8</v>
-      </c>
-      <c r="T1" t="s">
-        <v>9</v>
-      </c>
-      <c r="U1" t="s">
-        <v>10</v>
-      </c>
-      <c r="V1" t="s">
-        <v>11</v>
-      </c>
-      <c r="W1" t="s">
-        <v>12</v>
-      </c>
-      <c r="X1" t="s">
-        <v>13</v>
-      </c>
-      <c r="Y1" t="s">
-        <v>14</v>
-      </c>
-      <c r="Z1" t="s">
-        <v>15</v>
-      </c>
-      <c r="AA1" t="s">
-        <v>16</v>
-      </c>
-      <c r="AB1" t="s">
-        <v>17</v>
-      </c>
-      <c r="AC1" t="s">
-        <v>18</v>
-      </c>
-      <c r="AD1" t="s">
-        <v>19</v>
-      </c>
-      <c r="AE1" t="s">
-        <v>20</v>
-      </c>
-      <c r="AF1" t="s">
-        <v>21</v>
-      </c>
-      <c r="AG1" t="s">
-        <v>22</v>
-      </c>
-      <c r="AH1" t="s">
-        <v>23</v>
-      </c>
-      <c r="AI1" t="s">
-        <v>24</v>
-      </c>
-      <c r="AJ1" t="s">
-        <v>25</v>
-      </c>
-      <c r="AK1" t="s">
-        <v>26</v>
-      </c>
-      <c r="AL1" t="s">
-        <v>27</v>
-      </c>
-      <c r="AM1" t="s">
-        <v>28</v>
-      </c>
-      <c r="AN1" t="s">
-        <v>29</v>
-      </c>
-      <c r="AO1" t="s">
-        <v>30</v>
-      </c>
-      <c r="AP1" t="s">
-        <v>31</v>
-      </c>
-      <c r="AQ1" t="s">
-        <v>32</v>
-      </c>
-      <c r="AR1" t="s">
-        <v>33</v>
-      </c>
-      <c r="AS1" t="s">
-        <v>34</v>
-      </c>
-      <c r="AT1" t="s">
-        <v>35</v>
-      </c>
-      <c r="AU1" t="s">
-        <v>36</v>
-      </c>
-      <c r="AV1" t="s">
-        <v>37</v>
-      </c>
-      <c r="AW1" t="s">
-        <v>38</v>
-      </c>
-      <c r="AX1" t="s">
-        <v>39</v>
-      </c>
-      <c r="AY1" t="s">
-        <v>40</v>
-      </c>
-      <c r="AZ1" t="s">
-        <v>41</v>
-      </c>
-      <c r="BA1" t="s">
-        <v>42</v>
-      </c>
-      <c r="BB1" t="s">
-        <v>43</v>
+      <c r="BC1" t="s">
+        <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:54" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B2" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C2">
         <v>161605</v>
@@ -1369,6 +1405,66 @@
       <c r="BB2">
         <v>2.7E-2</v>
       </c>
+      <c r="BC2">
+        <v>45000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:55" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="2"/>
+      <c r="L3" s="2"/>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
+      <c r="U3" s="2"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="2"/>
+      <c r="Z3" s="2"/>
+      <c r="AA3" s="2"/>
+      <c r="AB3" s="2"/>
+      <c r="AC3" s="2"/>
+      <c r="AD3" s="2"/>
+      <c r="AE3" s="2"/>
+      <c r="AF3" s="2"/>
+      <c r="AG3" s="2"/>
+      <c r="AH3" s="2"/>
+      <c r="AI3" s="2"/>
+      <c r="AJ3" s="2"/>
+      <c r="AK3" s="2"/>
+      <c r="AL3" s="2"/>
+      <c r="AM3" s="2"/>
+      <c r="AN3" s="2"/>
+      <c r="AO3" s="2"/>
+      <c r="AP3" s="2"/>
+      <c r="AQ3" s="2"/>
+      <c r="AR3" s="2"/>
+      <c r="AS3" s="2"/>
+      <c r="AT3" s="2"/>
+      <c r="AU3" s="2"/>
+      <c r="AV3" s="2"/>
+      <c r="AW3" s="2"/>
+      <c r="AX3" s="2"/>
+      <c r="AY3" s="2"/>
+      <c r="AZ3" s="2"/>
+      <c r="BA3" s="2"/>
+      <c r="BB3" s="2"/>
+      <c r="BC3" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>